<commit_message>
add telas e finalizando soma total
</commit_message>
<xml_diff>
--- a/EXTRATO_TOTAL.xlsx
+++ b/EXTRATO_TOTAL.xlsx
@@ -358,7 +358,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F12"/>
+  <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -369,27 +369,37 @@
     <row r="1">
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>origem</t>
+          <t>nome</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>destino</t>
+          <t>preco</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>duracao</t>
+          <t>foto</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>conexao</t>
+          <t>ranking_site</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>preco</t>
+          <t>stars</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>url_site</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>endereco</t>
         </is>
       </c>
     </row>
@@ -399,27 +409,35 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>SSA - 06:10</t>
+          <t>Hotel Casa do Amarelindo</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>GRU - 08:40</t>
+          <t>R$ 458 - R$ 777</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 02:30</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> Direto </t>
-        </is>
+          <t>https://media-cdn.tripadvisor.com/media/photo-l/1c/bd/00/56/hotel-casa-do-amarelindo.jpg</t>
+        </is>
+      </c>
+      <c r="E2" t="n">
+        <v>4.8</v>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t xml:space="preserve"> R$ 1.480,45 </t>
+          <t>4.0</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>https://www.tripadvisor.com.br/Hotel_Review-g303272-d653336-Reviews-Hotel_Casa_do_Amarelindo-Salvador_State_of_Bahia.html</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>Rua das Portas do Carmo, 06 Pelourinho, Salvador, Bahia 40026-290 Brasil</t>
         </is>
       </c>
     </row>
@@ -429,27 +447,35 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>SSA - 11:15</t>
+          <t>Aram Yami Hotel</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>GRU - 13:45</t>
+          <t>R$ 1.022 - R$ 1.241</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 02:30</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> Direto </t>
-        </is>
+          <t>https://media-cdn.tripadvisor.com/media/photo-l/07/77/a3/75/aram-yami-hotel.jpg</t>
+        </is>
+      </c>
+      <c r="E3" t="n">
+        <v>4.78</v>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t xml:space="preserve"> R$ 1.480,45 </t>
+          <t>4.0</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>https://www.tripadvisor.com.br/Hotel_Review-g303272-d939414-Reviews-Aram_Yami_Hotel-Salvador_State_of_Bahia.html</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>Rua Direita de Santo Antônio 132 Santo Antonio Alem do Carmo, Salvador, Bahia 40301-280 Brasil</t>
         </is>
       </c>
     </row>
@@ -459,27 +485,35 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>SSA - 17:30</t>
+          <t>Hotel Fasano Salvador</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>GRU - 20:05</t>
+          <t>R$ 1.576 - R$ 2.199</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 02:35</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> Direto </t>
-        </is>
+          <t>https://media-cdn.tripadvisor.com/media/photo-l/1b/71/58/89/hotel-fasano-salvador.jpg</t>
+        </is>
+      </c>
+      <c r="E4" t="n">
+        <v>4.75</v>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t xml:space="preserve"> R$ 1.480,45 </t>
+          <t>4.5</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>https://www.tripadvisor.com.br/Hotel_Review-g303272-d15336700-Reviews-Hotel_Fasano_Salvador-Salvador_State_of_Bahia.html</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>Praça Castro Alves, 05, Salvador, Bahia 40020-160 Brasil</t>
         </is>
       </c>
     </row>
@@ -489,27 +523,35 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>SSA - 06:00</t>
+          <t>Monte Pascoal Praia Hotel</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>GRU - 12:40</t>
+          <t>R$ 426 - R$ 639</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 06:40</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> 1 parada </t>
-        </is>
+          <t>https://media-cdn.tripadvisor.com/media/photo-l/1c/40/41/9f/monte-pascoal-praia-hotel.jpg</t>
+        </is>
+      </c>
+      <c r="E5" t="n">
+        <v>4.68</v>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t xml:space="preserve"> R$ 2.523,45 </t>
+          <t>4.0</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>https://www.tripadvisor.com.br/Hotel_Review-g303272-d451517-Reviews-Monte_Pascoal_Praia_Hotel-Salvador_State_of_Bahia.html</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>Avenida Oceanica 591 Barra, Salvador, Bahia 40170-010 Brasil</t>
         </is>
       </c>
     </row>
@@ -519,207 +561,35 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>SSA - 09:15</t>
+          <t>Pousada Solar Dos Deuses</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>GRU - 13:50</t>
+          <t>R$ 431 - R$ 559</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 04:35</t>
-        </is>
-      </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> 1 parada </t>
-        </is>
+          <t>https://media-cdn.tripadvisor.com/media/photo-l/11/76/fd/c9/quarto-xango-com-balcao.jpg</t>
+        </is>
+      </c>
+      <c r="E6" t="n">
+        <v>4.63</v>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t xml:space="preserve"> R$ 2.523,45 </t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="1" t="n">
-        <v>5</v>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>SSA - 14:55</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>GRU - 19:30</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> 04:35</t>
-        </is>
-      </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> 1 parada </t>
-        </is>
-      </c>
-      <c r="F7" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> R$ 2.523,45 </t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="1" t="n">
-        <v>6</v>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>SSA - 15:10</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>GRU - 20:00</t>
-        </is>
-      </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> 04:50</t>
-        </is>
-      </c>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> 1 parada </t>
-        </is>
-      </c>
-      <c r="F8" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> R$ 2.523,45 </t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" s="1" t="n">
-        <v>7</v>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>SSA - 15:10</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>GRU - 20:10</t>
-        </is>
-      </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> 05:00</t>
-        </is>
-      </c>
-      <c r="E9" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> 1 parada </t>
-        </is>
-      </c>
-      <c r="F9" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> R$ 2.523,45 </t>
-        </is>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" s="1" t="n">
-        <v>8</v>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>SSA - 15:10</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>GRU - 21:35</t>
-        </is>
-      </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> 06:25</t>
-        </is>
-      </c>
-      <c r="E10" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> 1 parada </t>
-        </is>
-      </c>
-      <c r="F10" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> R$ 2.523,45 </t>
-        </is>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" s="1" t="n">
-        <v>9</v>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>SSA - 15:10</t>
-        </is>
-      </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>GRU - 22:45</t>
-        </is>
-      </c>
-      <c r="D11" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> 07:35</t>
-        </is>
-      </c>
-      <c r="E11" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> 1 parada </t>
-        </is>
-      </c>
-      <c r="F11" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> R$ 2.523,45 </t>
-        </is>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" s="1" t="n">
-        <v>10</v>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>SSA - 17:45</t>
-        </is>
-      </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>GRU - 22:45</t>
-        </is>
-      </c>
-      <c r="D12" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> 05:00</t>
-        </is>
-      </c>
-      <c r="E12" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> 1 parada </t>
-        </is>
-      </c>
-      <c r="F12" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> R$ 2.523,45 </t>
+          <t>3.5</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>https://www.tripadvisor.com.br/Hotel_Review-g303272-d1082005-Reviews-Pousada_Solar_Dos_Deuses-Salvador_State_of_Bahia.html</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>Largo Do Cruzeiro De São Francisco,12, Salvador, Bahia 40020-280 Brasil</t>
         </is>
       </c>
     </row>

</xml_diff>